<commit_message>
add final results used in presentation along with plots
</commit_message>
<xml_diff>
--- a/GenX_sims/sim1.3 - geothermal added/Generators_data.xlsx
+++ b/GenX_sims/sim1.3 - geothermal added/Generators_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/GenX/SCPA/Sim4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spenceregan/Repos/CU/Future_Power_Grid/Project2/GenX_sims/sim1.3 - geothermal added/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EC2C7EC-F2C6-7946-9EEB-DD97C5E0994D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6CE0BF-2797-1347-A1C0-16ACD33C91EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35400" yWindow="980" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="1840" yWindow="760" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generators_data" sheetId="1" r:id="rId1"/>
@@ -272,7 +272,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1106,12 +1106,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BK17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V9" sqref="V9"/>
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3220,6 +3220,38 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" spans="1:63" x14ac:dyDescent="0.2">
+      <c r="U14">
+        <f>U7+V7*48</f>
+        <v>145594</v>
+      </c>
+      <c r="X14">
+        <f>X7+Y7</f>
+        <v>10517</v>
+      </c>
+      <c r="AA14">
+        <f>AA7*12</f>
+        <v>1.7999999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:63" x14ac:dyDescent="0.2">
+      <c r="U15">
+        <f>U8+V8*96</f>
+        <v>279758</v>
+      </c>
+    </row>
+    <row r="16" spans="1:63" x14ac:dyDescent="0.2">
+      <c r="U16">
+        <f>U9+V9*8</f>
+        <v>349696</v>
+      </c>
+    </row>
+    <row r="17" spans="21:21" x14ac:dyDescent="0.2">
+      <c r="U17">
+        <f t="shared" ref="U15:U17" si="0">U10+V10*48</f>
+        <v>2026736</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>